<commit_message>
uodate get friend api
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V2.xlsx
+++ b/docs/API_Intro_V2.xlsx
@@ -547,24 +547,6 @@
   </si>
   <si>
     <t>{
- "status": 0,
- "server_friend_version",
- "friends": [
- { "nickname": xxxx,
-      "avatar_url": xxxx,
-      "mobile": xxx,
- },{}
- ]
- "circle": [
- { "circlename": xxx,
-      "circle_url": xxx,
- }, {}
- ]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
   "nickname": xxxx,
   "avatar_url": xxxx,
   "mobile": xxx,
@@ -637,7 +619,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>服务器判断mobile带来的version（1）到server的version（4),之间的number在服务器好友列表中都有对应，如果都有对应，那么将高于mobile version的好友类表带给mobile，否则要求mobile，获取所有的好友</t>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Push Message Format：
+msg content： 201
+extras： 发送方用户名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Push Message Format：
+msg content： 202
+extras： 发送方用户名</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -666,24 +660,31 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-服务器判断mobile带来的version（1）到server的version（4),之间的number在服务器好友列表中都有对应，如果都有对应，那么将高于mobile version的好友类表带给mobile，否则要求mobile，获取所有的好友</t>
+服务器判断mobile带来的version（1）到server的version（4),之间的number在服务器好友列表中都有对应，如果都有对应，那么将高于mobile version的好友类表带给mobile，否则将所有的好友列表返回给MOBILE</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>备注</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Push Message Format：
-msg content： 201
-extras： 发送方用户名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Push Message Format：
-msg content： 202
-extras： 发送方用户名</t>
+    <t>服务器判断mobile带来的version（1）到server的version（4),之间的number在服务器好友列表中都有对应，如果都有对应，那么将高于mobile version的好友类表带给mobile，否则将所有的好友列表返回给MOBILE</t>
+  </si>
+  <si>
+    <t>{
+ "status": 0,
+ "server_friend_version" :xxx,
+ "pdate_type: " 1 (全部更新)
+                2 （部分更新）
+ "friends": [
+ { "nickname": xxxx,
+      "avatar_url": xxxx,
+      "mobile": xxx,
+ },{}
+ ]
+ "circle": [
+ { "circlename": xxx,
+      "circle_url": xxx,
+ }, {}
+ ]
+}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1014,20 +1015,20 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1444,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1478,8 +1479,8 @@
       <c r="G2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="34" t="s">
-        <v>96</v>
+      <c r="H2" s="33" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.15">
@@ -1501,7 +1502,7 @@
       <c r="G3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="35"/>
+      <c r="H3" s="34"/>
     </row>
     <row r="4" spans="2:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="15"/>
@@ -1520,7 +1521,7 @@
       <c r="G4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="36"/>
+      <c r="H4" s="35"/>
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="2:9" ht="99.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -1540,7 +1541,7 @@
       <c r="G5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="37"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="2:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="13" t="s">
@@ -1561,8 +1562,8 @@
       <c r="G6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="35" t="s">
-        <v>97</v>
+      <c r="H6" s="34" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="96" customHeight="1" x14ac:dyDescent="0.15">
@@ -1577,11 +1578,11 @@
         <v>72</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="G7" s="25"/>
-      <c r="H7" s="36" t="s">
-        <v>98</v>
+      <c r="H7" s="35" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="96" customHeight="1" x14ac:dyDescent="0.15">
@@ -1593,13 +1594,13 @@
         <v>74</v>
       </c>
       <c r="E8" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="25" t="s">
-        <v>77</v>
-      </c>
       <c r="G8" s="25"/>
-      <c r="H8" s="36"/>
+      <c r="H8" s="35"/>
     </row>
     <row r="9" spans="2:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="2"/>
@@ -1618,7 +1619,7 @@
       <c r="G9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="36"/>
+      <c r="H9" s="35"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1739,8 +1740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1755,21 +1756,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="109.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F4" s="30"/>
       <c r="G4" s="32"/>
@@ -1778,7 +1779,7 @@
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="2:18" s="29" customFormat="1" x14ac:dyDescent="0.15"/>
@@ -1790,27 +1791,27 @@
         <v>66</v>
       </c>
       <c r="O7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
         <v>81</v>
       </c>
-      <c r="D8" t="s">
-        <v>82</v>
-      </c>
       <c r="H8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" t="s">
         <v>81</v>
       </c>
-      <c r="J8" t="s">
-        <v>82</v>
-      </c>
       <c r="O8" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q8" t="s">
         <v>81</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.15">
@@ -2083,7 +2084,7 @@
         <v>67</v>
       </c>
       <c r="O32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.15">
@@ -2201,7 +2202,7 @@
         <v>64</v>
       </c>
       <c r="O43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.15">
@@ -2233,10 +2234,10 @@
         <v>46</v>
       </c>
       <c r="H50" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O50" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.15">
@@ -2344,7 +2345,7 @@
     <row r="65" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="67" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B67" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.15">
@@ -2357,10 +2358,10 @@
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D69" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.15">
@@ -2379,7 +2380,7 @@
         <v>48</v>
       </c>
       <c r="D73" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.15">
@@ -2403,22 +2404,22 @@
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B80" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B82" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B85" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B87" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update get friend api
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V2.xlsx
+++ b/docs/API_Intro_V2.xlsx
@@ -355,14 +355,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>get friend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>friend/get_friend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">MOBILE </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -528,12 +520,6 @@
       "circle_url": xxx,
  }, {}
  ]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
- "mobile_friend_version": xxxx,
 }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -668,6 +654,17 @@
     <t>服务器判断mobile带来的version（1）到server的version（4),之间的number在服务器好友列表中都有对应，如果都有对应，那么将高于mobile version的好友类表带给mobile，否则将所有的好友列表返回给MOBILE</t>
   </si>
   <si>
+    <t>get friend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+"imsi":xxx
+"mobile_friend_version": xxxx,
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>{
  "status": 0,
  "server_friend_version" :xxx,
@@ -677,6 +674,8 @@
  { "nickname": xxxx,
       "avatar_url": xxxx,
       "mobile": xxx,
+      "status": 1,( 正常好友)
+                2( 待验证好友)
  },{}
  ]
  "circle": [
@@ -685,6 +684,10 @@
  }, {}
  ]
 }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>friend/get_friend</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1446,7 +1449,7 @@
   <dimension ref="B2:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1480,7 +1483,7 @@
         <v>26</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.15">
@@ -1563,41 +1566,41 @@
         <v>24</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="96" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G7" s="25"/>
       <c r="H7" s="35" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="96" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="25" t="s">
         <v>73</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>76</v>
       </c>
       <c r="G8" s="25"/>
       <c r="H8" s="35"/>
@@ -1614,7 +1617,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>23</v>
@@ -1757,7 +1760,7 @@
   <sheetData>
     <row r="1" spans="2:18" ht="109.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="37" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
@@ -1765,12 +1768,12 @@
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F4" s="30"/>
       <c r="G4" s="32"/>
@@ -1779,521 +1782,521 @@
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="2:18" s="29" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="7" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="Q8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B11" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O11" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q11" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B13" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O13" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q13" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B15" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="H15" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" t="s">
         <v>50</v>
       </c>
-      <c r="E15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H15" s="19" t="s">
+      <c r="O15" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q15" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="R15" t="s">
         <v>50</v>
-      </c>
-      <c r="J15" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="K15" t="s">
-        <v>52</v>
-      </c>
-      <c r="O15" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q15" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="R15" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B18" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C18" s="26"/>
       <c r="D18" s="26"/>
       <c r="E18" s="26"/>
       <c r="H18" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
       <c r="K18" s="26"/>
       <c r="N18" s="26"/>
       <c r="O18" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.15">
       <c r="H20" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" t="s">
         <v>43</v>
       </c>
-      <c r="J20" t="s">
-        <v>45</v>
-      </c>
       <c r="O20" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q20" t="s">
         <v>43</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B21" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B23" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D23" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" t="s">
         <v>49</v>
       </c>
-      <c r="E23" t="s">
-        <v>51</v>
-      </c>
       <c r="H23" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O23" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q23" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B25" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" t="s">
-        <v>52</v>
-      </c>
       <c r="H25" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J25" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="K25" t="s">
         <v>49</v>
       </c>
-      <c r="K25" t="s">
-        <v>51</v>
-      </c>
       <c r="O25" s="27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q25" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.15">
       <c r="D27" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H27" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J27" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="K27" t="s">
         <v>50</v>
       </c>
-      <c r="J27" s="19" t="s">
+      <c r="O27" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q27" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="R27" t="s">
         <v>50</v>
-      </c>
-      <c r="K27" t="s">
-        <v>52</v>
-      </c>
-      <c r="O27" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q27" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="R27" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O32" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B34" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.15">
       <c r="H35" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="O35" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.15">
       <c r="H37" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I37" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J37" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K37" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O37" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q37" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R37" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B39" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H39" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="I39" t="s">
         <v>49</v>
       </c>
-      <c r="I39" t="s">
-        <v>51</v>
-      </c>
       <c r="J39" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="K39" t="s">
         <v>49</v>
       </c>
-      <c r="K39" t="s">
-        <v>51</v>
-      </c>
       <c r="O39" s="27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q39" s="27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R39" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H41" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I41" t="s">
         <v>50</v>
       </c>
-      <c r="I41" t="s">
-        <v>52</v>
-      </c>
       <c r="J41" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="K41" t="s">
+        <v>68</v>
+      </c>
+      <c r="O41" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q41" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="R41" t="s">
         <v>50</v>
-      </c>
-      <c r="K41" t="s">
-        <v>70</v>
-      </c>
-      <c r="O41" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q41" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="R41" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="42" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H42" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O42" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B43" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O43" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.15">
       <c r="H44" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B45" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B48" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D48" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B50" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E50" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H50" s="22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="O50" s="22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B52" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E52" t="s">
         <v>49</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E52" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.15">
       <c r="H53" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B54" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E54" t="s">
         <v>50</v>
       </c>
-      <c r="D54" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E54" t="s">
-        <v>52</v>
-      </c>
       <c r="H54" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J54" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B56" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E56" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H56" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I56" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J56" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K56" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.15">
@@ -2316,80 +2319,80 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.15">
       <c r="H58" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="I58" t="s">
         <v>49</v>
       </c>
-      <c r="I58" t="s">
-        <v>51</v>
-      </c>
       <c r="J58" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="K58" t="s">
         <v>49</v>
-      </c>
-      <c r="K58" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.15">
       <c r="H60" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I60" t="s">
         <v>50</v>
       </c>
-      <c r="I60" t="s">
-        <v>52</v>
-      </c>
       <c r="J60" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K60" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="67" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B67" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B68" t="s">
+        <v>41</v>
+      </c>
+      <c r="D68" t="s">
         <v>43</v>
-      </c>
-      <c r="D68" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B69" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D69" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B71" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D71" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E71" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B73" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D73" s="27" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.15">
       <c r="C75" s="28"/>
       <c r="D75" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E75" t="s">
         <v>50</v>
-      </c>
-      <c r="E75" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.15">
@@ -2404,22 +2407,22 @@
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B80" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B82" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B85" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B87" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[add friend]return server friend version
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V2.xlsx
+++ b/docs/API_Intro_V2.xlsx
@@ -351,12 +351,6 @@
     <t>undefine error</t>
   </si>
   <si>
-    <t>{
- "status": 0
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">MOBILE </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -856,6 +850,36 @@
         <scheme val="minor"/>
       </rPr>
       <t>}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{
+ "status": 0
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"server_friend_version": xxx,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+}</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1628,7 +1652,7 @@
   <dimension ref="B2:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1662,7 +1686,7 @@
         <v>24</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.15">
@@ -1695,7 +1719,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>15</v>
@@ -1736,52 +1760,52 @@
         <v>11</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="2"/>
       <c r="C7" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>94</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G7" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7" s="35" t="s">
         <v>89</v>
-      </c>
-      <c r="H7" s="35" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="173.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>88</v>
-      </c>
       <c r="E8" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G8" s="37"/>
       <c r="H8" s="35"/>
@@ -1789,16 +1813,16 @@
     <row r="9" spans="2:9" ht="96" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="D9" s="24" t="s">
-        <v>96</v>
-      </c>
       <c r="E9" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G9" s="25"/>
       <c r="H9" s="35"/>
@@ -1812,10 +1836,10 @@
         <v>13</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>21</v>
@@ -1958,7 +1982,7 @@
   <sheetData>
     <row r="1" spans="2:18" ht="109.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C1" s="38"/>
       <c r="D1" s="38"/>
@@ -1966,12 +1990,12 @@
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" s="30"/>
       <c r="G4" s="32"/>
@@ -1980,521 +2004,521 @@
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="2:18" s="29" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="7" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" t="s">
         <v>70</v>
       </c>
-      <c r="D8" t="s">
-        <v>71</v>
-      </c>
       <c r="H8" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" t="s">
         <v>70</v>
       </c>
-      <c r="J8" t="s">
-        <v>71</v>
-      </c>
       <c r="O8" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q8" t="s">
         <v>70</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B11" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="19" t="s">
-        <v>42</v>
-      </c>
       <c r="J11" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K11" t="s">
+        <v>40</v>
+      </c>
+      <c r="O11" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="O11" s="19" t="s">
-        <v>42</v>
-      </c>
       <c r="Q11" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B13" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O13" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q13" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B15" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J15" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O15" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q15" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B18" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" s="26"/>
       <c r="D18" s="26"/>
       <c r="E18" s="26"/>
       <c r="H18" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
       <c r="K18" s="26"/>
       <c r="N18" s="26"/>
       <c r="O18" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.15">
       <c r="H20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B21" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B23" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="19" t="s">
-        <v>44</v>
-      </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K23" t="s">
+        <v>40</v>
+      </c>
+      <c r="O23" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="O23" s="19" t="s">
-        <v>42</v>
-      </c>
       <c r="Q23" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B25" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" t="s">
+        <v>46</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="J25" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K25" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="O25" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q25" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="R25" t="s">
         <v>45</v>
-      </c>
-      <c r="E25" t="s">
-        <v>47</v>
-      </c>
-      <c r="H25" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="J25" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="K25" t="s">
-        <v>46</v>
-      </c>
-      <c r="O25" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q25" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="R25" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.15">
       <c r="D27" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" t="s">
         <v>48</v>
       </c>
-      <c r="E27" t="s">
-        <v>49</v>
-      </c>
       <c r="H27" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J27" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O27" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q27" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.15">
       <c r="H35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.15">
       <c r="H37" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I37" t="s">
+        <v>40</v>
+      </c>
+      <c r="J37" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="J37" s="19" t="s">
-        <v>42</v>
-      </c>
       <c r="K37" t="s">
+        <v>40</v>
+      </c>
+      <c r="O37" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="O37" s="19" t="s">
-        <v>42</v>
-      </c>
       <c r="Q37" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J39" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O39" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q39" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H41" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J41" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O41" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q41" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.15">
       <c r="H44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B50" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H50" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O50" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B52" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.15">
       <c r="H53" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B54" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E54" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B56" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E56" t="s">
         <v>48</v>
       </c>
-      <c r="D56" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E56" t="s">
-        <v>49</v>
-      </c>
       <c r="H56" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I56" t="s">
+        <v>40</v>
+      </c>
+      <c r="J56" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="J56" s="19" t="s">
-        <v>42</v>
-      </c>
       <c r="K56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.15">
@@ -2517,80 +2541,80 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.15">
       <c r="H58" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I58" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J58" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K58" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.15">
       <c r="H60" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I60" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J60" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="67" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B68" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D68" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B69" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D69" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B71" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D71" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E71" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B73" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D73" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.15">
       <c r="C75" s="28"/>
       <c r="D75" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E75" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.15">
@@ -2605,22 +2629,22 @@
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B80" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B82" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B85" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B87" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the parameters that dealing with friend
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V2.xlsx
+++ b/docs/API_Intro_V2.xlsx
@@ -530,23 +530,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{
- "status": 0,
- "friends": [
- { "nickname": xxxx,
-      "avatar_url": xxxx,
-      "mobile": xxx,
- },{}
- ]
- "circle": [
- { "circlename": xxx,
-      "circle_url": xxx,
- }, {}
- ]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MOBILE 将FRIEND 2的删除事件上报server</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -702,84 +685,6 @@
   </si>
   <si>
     <t>friend/update_friend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
- "imsi": xxxx,  //my imsi 
- "target_user": xxxx,
- "comment": xxxx,
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">{
- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"client": xxxx</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
- "search_str": xxxx,
-}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-"client":xxx
-"imsi":xxx
-"mobile_friend_version": xxxx,
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">{
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "client": xxxx,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
- "nok": x, //1: agree, 0: disagree
- "imsi": xxxx,
- "target_user": xxxx,
-}</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -818,38 +723,6 @@
   <si>
     <r>
       <t xml:space="preserve">{
-  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"client": xxx,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-  "nickname": xxxx,
-  "avatar_url": xxxx,
-  "mobile": xxx,
-}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">{
  "mobile": xxxx,
  "password": xxxx,
  "confirmpass": xxxx,
@@ -920,8 +793,98 @@
   </si>
   <si>
     <t>{
-  "client": xxx,
-  "mobile": xxx,
+ /* the mobile that register */
+ "mobile": xxxx,
+ /* the mobile that want to add */
+ "add friend": xxxx, 
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> /* the mobile that register */
+ "mobile": xxxx,
+ /* 1: agree, 0: disagree */</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ "nok": x,
+ /* the mobile that want to respone */
+ "to friend": xxxx, 
+}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ /* the mobile that register */
+ "mobile": xxxx,
+ "mobile_friend_version": xxxx,
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ /* the mobile that register */
+ "mobile": xxxx,
+ /* comment to identify friend */
+ "comment": xxxx,
+ /* group that settle the friend */
+ "group": xxxx,
+ /* description for friend */
+ "description": xxxx,
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ /* the mobile that register */
+ "mobile": xxxx,
+ /* the mobile that want to delete */
+ "delete friend": xxxx, 
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ /* the mobile that register */
+ "mobile": xxxx,
+ "search_str": xxxx,
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "status": 0,
+ "friends": [
+ { "nickname": xxxx,
+      "avatar_url": xxxx,
+      "mobile": xxx,
+ },{}
+ ]
+ "circle": [
+ { "circlename": xxx,
+      "circle_url": xxx,
+ }, {}
+ ]
 }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1294,9 +1257,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1309,6 +1269,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1726,7 +1689,7 @@
   <dimension ref="B2:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1734,7 +1697,7 @@
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="21.5" style="12" customWidth="1"/>
     <col min="4" max="4" width="27.75" style="12" customWidth="1"/>
-    <col min="5" max="5" width="25" style="22" customWidth="1"/>
+    <col min="5" max="5" width="39.25" style="22" customWidth="1"/>
     <col min="6" max="6" width="33.25" style="22" customWidth="1"/>
     <col min="7" max="7" width="56.375" customWidth="1"/>
     <col min="8" max="8" width="56.375" style="17" customWidth="1"/>
@@ -1760,7 +1723,7 @@
         <v>24</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="99.95" customHeight="1">
@@ -1793,7 +1756,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>15</v>
@@ -1834,52 +1797,52 @@
         <v>11</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="99.95" customHeight="1">
       <c r="B7" s="2"/>
       <c r="C7" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>93</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G7" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="35" t="s">
         <v>88</v>
-      </c>
-      <c r="H7" s="35" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="173.25" customHeight="1">
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>87</v>
-      </c>
       <c r="E8" s="25" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G8" s="37"/>
       <c r="H8" s="35"/>
@@ -1887,36 +1850,36 @@
     <row r="9" spans="2:9" ht="96" customHeight="1">
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="24" t="s">
-        <v>95</v>
-      </c>
       <c r="E9" s="25" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G9" s="25"/>
       <c r="H9" s="35"/>
     </row>
-    <row r="10" spans="2:9" s="40" customFormat="1" ht="96" customHeight="1">
-      <c r="B10" s="41"/>
-      <c r="C10" s="42" t="s">
+    <row r="10" spans="2:9" s="39" customFormat="1" ht="96" customHeight="1">
+      <c r="B10" s="40"/>
+      <c r="C10" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="E10" s="43" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="G10" s="43"/>
-      <c r="H10" s="39"/>
+      <c r="F10" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" s="42"/>
+      <c r="H10" s="38"/>
     </row>
     <row r="11" spans="2:9" ht="83.25" customHeight="1">
       <c r="B11" s="2"/>
@@ -1927,10 +1890,10 @@
         <v>13</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>21</v>
@@ -2072,21 +2035,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="109.5" customHeight="1">
-      <c r="B1" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="B1" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="3" spans="2:18">
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="2:18">
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" s="30"/>
       <c r="G4" s="32"/>
@@ -2095,7 +2058,7 @@
     </row>
     <row r="5" spans="2:18">
       <c r="B5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="2:18" s="29" customFormat="1"/>
@@ -2107,27 +2070,27 @@
         <v>60</v>
       </c>
       <c r="O7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="2:18">
       <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
         <v>69</v>
       </c>
-      <c r="D8" t="s">
-        <v>70</v>
-      </c>
       <c r="H8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" t="s">
         <v>69</v>
       </c>
-      <c r="J8" t="s">
-        <v>70</v>
-      </c>
       <c r="O8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q8" t="s">
         <v>69</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="9" spans="2:18">
@@ -2400,7 +2363,7 @@
         <v>61</v>
       </c>
       <c r="O32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="2:18">
@@ -2518,7 +2481,7 @@
         <v>58</v>
       </c>
       <c r="O43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="2:18">
@@ -2550,10 +2513,10 @@
         <v>40</v>
       </c>
       <c r="H50" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O50" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:18">
@@ -2661,7 +2624,7 @@
     <row r="65" spans="2:5" s="29" customFormat="1"/>
     <row r="67" spans="2:5">
       <c r="B67" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="2:5">
@@ -2674,10 +2637,10 @@
     </row>
     <row r="69" spans="2:5">
       <c r="B69" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D69" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="2:5">
@@ -2696,7 +2659,7 @@
         <v>42</v>
       </c>
       <c r="D73" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="2:5">
@@ -2720,22 +2683,22 @@
     </row>
     <row r="80" spans="2:5">
       <c r="B80" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="82" spans="2:2">
       <c r="B82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="85" spans="2:2">
       <c r="B85" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="87" spans="2:2">
       <c r="B87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>